<commit_message>
added matlab stuff for sensitivity study
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -27,6 +27,7 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
+            <charset val="1"/>
             <family val="2"/>
             <b val="true"/>
             <color rgb="00000000"/>
@@ -38,6 +39,7 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
+            <charset val="1"/>
             <family val="2"/>
             <color rgb="00000000"/>
             <sz val="9"/>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="187">
   <si>
     <t>My BRNS Tests</t>
   </si>
@@ -326,6 +328,12 @@
     <t>40.0e-9</t>
   </si>
   <si>
+    <t>500m + anoxic, no Fe, no Mn</t>
+  </si>
+  <si>
+    <t>Test 4_1</t>
+  </si>
+  <si>
     <t>5000m + oxic + all species</t>
   </si>
   <si>
@@ -446,7 +454,19 @@
     <t>rate22:= kpyr*fes*(h2s+hs);</t>
   </si>
   <si>
+    <t>Setup 1</t>
+  </si>
+  <si>
+    <t>oxic, 5000m, 0.1 wt% at SWI</t>
+  </si>
+  <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>Setup 2</t>
+  </si>
+  <si>
+    <t>anoxic, 500m, 1.0 wt% at SWI</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -494,6 +514,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -518,6 +539,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -528,6 +550,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -555,6 +578,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -565,6 +589,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -613,6 +638,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -631,6 +657,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -691,6 +718,7 @@
   <fonts count="15">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -711,24 +739,28 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -736,6 +768,7 @@
     </font>
     <font>
       <name val="arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -743,11 +776,13 @@
     </font>
     <font>
       <name val="arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -755,12 +790,14 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00FF0000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -768,6 +805,7 @@
     </font>
     <font>
       <name val="Verdana"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00000000"/>
@@ -775,6 +813,7 @@
     </font>
     <font>
       <name val="Verdana"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="9"/>
@@ -834,7 +873,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -854,8 +893,6 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
@@ -871,9 +908,6 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -960,29 +994,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AY55"/>
+  <dimension ref="A2:AY56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="J26" activeCellId="0" pane="topLeft" sqref="J26"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.443137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.64313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="38.9450980392157"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.2470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.9843137254902"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2470588235294"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.2901960784314"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.1333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.756862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3490196078431"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.75294117647059"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.5254901960784"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.5019607843137"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.2745098039216"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5019607843137"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.5882352941177"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.5137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -1819,6 +1853,9 @@
       <c r="AX10" s="15" t="n">
         <v>0.00010417</v>
       </c>
+      <c r="AY10" s="3" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
@@ -1827,69 +1864,69 @@
       <c r="C11" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E11" s="0" t="n">
+      <c r="D11" s="3" t="n">
+        <v>500</v>
+      </c>
+      <c r="E11" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="F11" s="6" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G11" s="9" t="n">
+      <c r="F11" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="13" t="n">
         <f aca="false">E11/J11</f>
-        <v>34030.609703112</v>
-      </c>
-      <c r="H11" s="6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="I11" s="0" t="n">
+        <v>374.826018814378</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="I11" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="J11" s="10" t="n">
+      <c r="J11" s="14" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D11)</f>
-        <v>0.00293853095411498</v>
-      </c>
-      <c r="K11" s="6" t="n">
+        <v>0.266790444047381</v>
+      </c>
+      <c r="K11" s="3" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D11))</f>
-        <v>0.310744423452098</v>
-      </c>
-      <c r="L11" s="0" t="n">
+        <v>19.0459808634568</v>
+      </c>
+      <c r="L11" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="3" t="n">
         <v>0.85</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="6" t="n">
-        <v>0.0122</v>
-      </c>
-      <c r="P11" s="0" t="n">
+      <c r="O11" s="3" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="P11" s="3" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q11" s="7" t="n">
+      <c r="Q11" s="15" t="n">
         <v>8E-009</v>
       </c>
-      <c r="R11" s="6" t="n">
+      <c r="R11" s="0" t="n">
         <f aca="false">S11/(100*12)*2.5</f>
-        <v>1.04166666666667E-005</v>
-      </c>
-      <c r="S11" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="V11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="W11" s="8" t="s">
-        <v>82</v>
+        <v>0.000104166666666667</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>83</v>
@@ -1969,214 +2006,370 @@
       <c r="AW11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="AX11" s="6" t="n">
-        <f aca="false">AY11/(100*12)*2.5</f>
+      <c r="AX11" s="15" t="n">
+        <v>0.00010417</v>
+      </c>
+      <c r="AY11" s="3" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="B12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G12" s="9" t="n">
+        <f aca="false">E12/J12</f>
+        <v>34030.6097031119</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">3.3*10^(-0.87478367-0.00043512*D12)</f>
+        <v>0.00293853095411498</v>
+      </c>
+      <c r="K12" s="6" t="n">
+        <f aca="false">5.2*(10^(0.7624-0.0003972*D12))</f>
+        <v>0.310744423452098</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <v>8E-009</v>
+      </c>
+      <c r="R12" s="6" t="n">
+        <f aca="false">S12/(100*12)*2.5</f>
         <v>1.04166666666667E-005</v>
       </c>
-      <c r="AY11" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
-      <c r="B16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="S12" s="11" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="B17" s="0" t="s">
+      <c r="T12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM12" s="3" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="AN12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="6" t="n">
+        <f aca="false">AY12/(100*12)*2.5</f>
+        <v>1.04166666666667E-005</v>
+      </c>
+      <c r="AY12" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
+      <c r="B17" s="4" t="s">
         <v>96</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="B23" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="B28" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="B27" s="0" t="s">
         <v>107</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="B29" s="0" t="s">
         <v>108</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="B31" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="B32" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="B34" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
-      <c r="B36" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="B37" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="B38" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="B39" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="B40" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
-      <c r="B42" s="0" t="s">
         <v>118</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="B41" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="B43" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="B45" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="B46" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="B47" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="B48" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
-      <c r="B50" s="0" t="s">
         <v>125</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="B49" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="B51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="B52" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="B53" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="B54" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="B55" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="B56" s="0" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2195,129 +2388,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C29" activeCellId="0" pane="topLeft" sqref="C29"/>
+      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.8823529411765"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.9843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
+      <c r="B2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
-      <c r="B3" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="16" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
+      <c r="B3" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="C3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
+      <c r="B5" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
-      <c r="B4" s="16" t="s">
+      <c r="C5" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="6">
+      <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="18" t="n">
+      <c r="C6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="7" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F6" s="17" t="n">
         <v>50</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
-      <c r="B5" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="21" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F5" s="22" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="6">
-      <c r="B6" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1.7</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="23" t="n">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="18.65" outlineLevel="0" r="7">
-      <c r="A7" s="24" t="s">
+      <c r="H6" s="18" t="s">
         <v>148</v>
       </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="B7" s="16" t="s">
         <v>149</v>
       </c>
@@ -2325,224 +2496,267 @@
         <v>150</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="20" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="8">
+      <c r="B8" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H8" s="21" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="9">
+      <c r="A9" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="18.65" outlineLevel="0" r="8">
-      <c r="A8" s="24" t="s">
+      <c r="G9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="10">
+      <c r="A10" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="23" t="n">
+      <c r="G10" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="21" t="n">
         <v>1.3</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
-      <c r="B9" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="I10" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
+      <c r="B11" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
         <v>43.8</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <f aca="false">0.1*24*365</f>
         <v>876</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H9" s="23" t="n">
+      <c r="G11" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="21" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
-      <c r="B10" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="0" t="n">
+      <c r="I11" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
+      <c r="B12" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
         <v>0.015768</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F12" s="0" t="n">
         <f aca="false">2.2*10^{-6}*24*365</f>
         <v>0.019272</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="25" t="n">
+      <c r="G12" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="H12" s="23" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
-      <c r="B11" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H11" s="23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="12">
-      <c r="A12" s="24" t="s">
+      <c r="I12" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="23" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="13">
-      <c r="B13" s="4" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
+      <c r="B13" s="16" t="s">
         <v>168</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="D13" s="0" t="s">
+        <v>146</v>
+      </c>
       <c r="E13" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" s="21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="14">
+      <c r="A14" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="23" t="n">
+      <c r="H14" s="21" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="15">
+      <c r="B15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="21" t="n">
         <v>0.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="H14" s="23"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="H15" s="23"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="B16" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H16" s="23"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
-      <c r="B17" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="H17" s="26" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="H16" s="21"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="H17" s="21"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="B18" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H18" s="21"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
+      <c r="B19" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H19" s="18" t="n">
         <f aca="false">1*10^{-9}</f>
         <v>1E-009</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
-      <c r="B18" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="H18" s="27" t="n">
+      <c r="I19" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
+      <c r="B20" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="24" t="n">
         <f aca="false">3.7*10^{-9}</f>
         <v>3.7E-009</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
-      <c r="C21" s="0" t="s">
-        <v>176</v>
+      <c r="I20" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="C23" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2564,17 +2778,17 @@
   <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0039215686275"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.9960784313725"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -2582,59 +2796,59 @@
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="16" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" s="29"/>
+        <v>143</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="19" t="n">
+        <v>146</v>
+      </c>
+      <c r="E4" s="17" t="n">
         <v>6E-007</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F4" s="17" t="n">
         <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" s="30" t="n">
+        <v>147</v>
+      </c>
+      <c r="H4" s="27" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="I4" s="29" t="n">
+      <c r="I4" s="26" t="n">
         <v>50</v>
       </c>
     </row>
@@ -2643,52 +2857,52 @@
         <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="19" t="n">
+        <v>146</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="30" t="n">
+        <v>147</v>
+      </c>
+      <c r="H5" s="27" t="n">
         <f aca="false">1*10^{-6}</f>
         <v>1E-006</v>
       </c>
-      <c r="I5" s="30" t="n">
+      <c r="I5" s="27" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="6">
       <c r="B6" s="16" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="7">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>250</v>
@@ -2697,16 +2911,16 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
-      <c r="A8" s="24" t="s">
-        <v>148</v>
+      <c r="A8" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="B8" s="16"/>
       <c r="D8" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>108</v>
@@ -2715,21 +2929,21 @@
         <v>243</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="9">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1.3</v>
@@ -2738,30 +2952,30 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
-      <c r="A10" s="24" t="s">
-        <v>148</v>
+      <c r="A10" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="B10" s="16"/>
       <c r="D10" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="B11" s="16" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -2772,25 +2986,25 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="B12" s="16" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -2801,25 +3015,25 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H12" s="31" t="n">
+        <v>164</v>
+      </c>
+      <c r="H12" s="28" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="16" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">1*10^{-6}*24*365</f>
@@ -2830,25 +3044,25 @@
         <v>4.38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H13" s="3" t="n">
         <f aca="false">365*1*10^{-3}</f>
         <v>0.365</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="B14" s="16" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.001</v>
@@ -2857,40 +3071,40 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="16" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="16" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
+      <c r="A17" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
-      <c r="A17" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.5</v>
@@ -2901,10 +3115,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="18">
       <c r="B18" s="4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.5</v>
@@ -2915,7 +3129,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more stuff for sensitivity study w and Dbio not depth related
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -2390,8 +2390,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -2401,7 +2401,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9294117647059"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3450980392157"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6509803921569"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3058823529412"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9294117647059"/>
   </cols>

</xml_diff>

<commit_message>
added some folder Two_fractions/OMEN-BRNS
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="189">
   <si>
     <t>My BRNS Tests</t>
   </si>
@@ -466,7 +466,7 @@
     <t>Setup 2</t>
   </si>
   <si>
-    <t>anoxic, 500m, 1.0 wt% at SWI</t>
+    <t>anoxic (O2, NO3 as with BRNS), 500m, 1.0 wt% at SWI</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -689,6 +689,12 @@
   </si>
   <si>
     <t>Latin-Hypercube: n &gt;= 10 x parameters</t>
+  </si>
+  <si>
+    <t>Setup 1 problems</t>
+  </si>
+  <si>
+    <t>Setup 2 problems</t>
   </si>
   <si>
     <t>Would vary OM degradation from</t>
@@ -996,27 +1002,27 @@
   </sheetPr>
   <dimension ref="A2:AY56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.756862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.75294117647059"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.5254901960784"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.5019607843137"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.2745098039216"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5019607843137"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.5882352941177"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.5137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.721568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.5921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3725490196078"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5921568627451"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.6823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.6392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -2388,22 +2394,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
+      <selection activeCell="C29" activeCellId="0" pane="topLeft" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6509803921569"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3058823529412"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.4980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.8352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4039215686274"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
@@ -2757,6 +2763,29 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="B31" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="B32" s="0" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="B33" s="0" t="n">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2782,13 +2811,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.9960784313725"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.5254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -2821,7 +2850,7 @@
         <v>143</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I3" s="26"/>
     </row>
@@ -2857,7 +2886,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>146</v>
@@ -2911,7 +2940,7 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
@@ -2952,7 +2981,7 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
@@ -3129,7 +3158,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date to matlab plot functions + output in apropriate directory
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="190">
   <si>
     <t>My BRNS Tests</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>rate22:= kpyr*fes*(h2s+hs);</t>
+  </si>
+  <si>
+    <t>Tmp 8.1</t>
   </si>
   <si>
     <t>Setup 1</t>
@@ -1003,26 +1006,22 @@
   <dimension ref="A2:AY56"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
+      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8470588235294"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.79607843137255"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.721568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.5921568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3725490196078"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5921568627451"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.6823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.6392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9254901960784"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83137254901961"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6823529411765"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4705882352941"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.6823529411765"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7803921568627"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.7686274509804"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -2397,42 +2396,41 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C29" activeCellId="0" pane="topLeft" sqref="C29"/>
+      <selection activeCell="E27" activeCellId="0" pane="topLeft" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.4980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.8352941176471"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4039215686274"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="B2" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2449,25 +2447,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="B5" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="6">
@@ -2475,10 +2473,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E6" s="7" t="n">
         <f aca="false">1*10^{-3}</f>
@@ -2488,21 +2486,21 @@
         <v>50</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="B7" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="E7" s="19" t="n">
         <v>0.05</v>
@@ -2511,15 +2509,15 @@
         <v>0.95</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="8">
       <c r="B8" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0.8</v>
@@ -2528,7 +2526,7 @@
         <v>1.7</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H8" s="21" t="n">
         <v>1.3</v>
@@ -2536,16 +2534,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="9">
       <c r="A9" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>100</v>
@@ -2554,27 +2552,27 @@
         <v>400</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="10">
       <c r="A10" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1.3</v>
@@ -2583,24 +2581,24 @@
         <v>2</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H10" s="21" t="n">
         <v>1.3</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="B11" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -2611,25 +2609,25 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H11" s="21" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="B12" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -2640,25 +2638,25 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H12" s="23" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.001</v>
@@ -2667,7 +2665,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H13" s="21" t="n">
         <v>1</v>
@@ -2675,13 +2673,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="14">
       <c r="A14" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.5</v>
@@ -2695,10 +2693,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="15">
       <c r="B15" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.5</v>
@@ -2718,72 +2716,72 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H18" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="B19" s="16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H19" s="18" t="n">
         <f aca="false">1*10^{-9}</f>
         <v>1E-009</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
       <c r="B20" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="H20" s="24" t="n">
         <f aca="false">3.7*10^{-9}</f>
         <v>3.7E-009</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
+        <v>183</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+        <v>185</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="B31" s="0" t="n">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="B32" s="0" t="n">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="0" t="n">
         <v>164</v>
       </c>
@@ -2811,13 +2809,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2235294117647"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.5254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.6549019607843"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -2825,32 +2821,32 @@
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I3" s="26"/>
     </row>
@@ -2859,10 +2855,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E4" s="17" t="n">
         <v>6E-007</v>
@@ -2871,7 +2867,7 @@
         <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H4" s="27" t="n">
         <f aca="false">1*10^{-3}</f>
@@ -2886,10 +2882,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E5" s="17" t="n">
         <v>0</v>
@@ -2898,7 +2894,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H5" s="27" t="n">
         <f aca="false">1*10^{-6}</f>
@@ -2911,27 +2907,27 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="6">
       <c r="B6" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="7">
       <c r="A7" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>250</v>
@@ -2940,16 +2936,16 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" s="16"/>
       <c r="D8" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>108</v>
@@ -2958,21 +2954,21 @@
         <v>243</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="9">
       <c r="A9" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1.3</v>
@@ -2981,30 +2977,30 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B10" s="16"/>
       <c r="D10" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="B11" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -3015,25 +3011,25 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="B12" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -3044,25 +3040,25 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H12" s="28" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">1*10^{-6}*24*365</f>
@@ -3073,25 +3069,25 @@
         <v>4.38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H13" s="3" t="n">
         <f aca="false">365*1*10^{-3}</f>
         <v>0.365</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="B14" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.001</v>
@@ -3100,40 +3096,40 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
       <c r="A17" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.5</v>
@@ -3144,10 +3140,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="18">
       <c r="B18" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.5</v>
@@ -3158,7 +3154,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rest of comments Sandra
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="212" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="243" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="OMEN-BRNS" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="191">
   <si>
     <t>My BRNS Tests</t>
   </si>
@@ -674,6 +674,9 @@
   </si>
   <si>
     <t>include these as well? Which range?</t>
+  </si>
+  <si>
+    <t>' +/- 50%</t>
   </si>
   <si>
     <t>PO4s</t>
@@ -1005,23 +1008,29 @@
   </sheetPr>
   <dimension ref="A2:AY56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
+      <selection activeCell="F25" activeCellId="0" pane="topLeft" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4745098039216"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4705882352941"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7803921568627"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.7686274509804"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6823529411765"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.94901960784314"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.5176470588235"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.9529411764706"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.7607843137255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.9529411764706"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -2395,16 +2404,20 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E27" activeCellId="0" pane="topLeft" sqref="E27"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
+      <selection activeCell="C28" activeCellId="0" pane="topLeft" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6509803921569"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.556862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
@@ -2721,14 +2734,17 @@
       <c r="H18" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="B19" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H19" s="18" t="n">
         <f aca="false">1*10^{-9}</f>
@@ -2739,14 +2755,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="B20" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>180</v>
       </c>
       <c r="H20" s="24" t="n">
         <f aca="false">3.7*10^{-9}</f>
@@ -2760,15 +2779,15 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
@@ -2804,16 +2823,18 @@
   </sheetPr>
   <dimension ref="A2:I21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
       <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.6549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1058823529412"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.0509803921569"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.63921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -2846,7 +2867,7 @@
         <v>144</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I3" s="26"/>
     </row>
@@ -2882,7 +2903,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>147</v>
@@ -2936,7 +2957,7 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
@@ -2977,7 +2998,7 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
@@ -3101,24 +3122,24 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
@@ -3154,7 +3175,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBSA save all outpus and create/save figures as .eps make Sens-index plot for different outputs and different parameters
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="249">
   <si>
     <t>Thullner et al. 2009</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>PO4</t>
+  </si>
+  <si>
+    <t>zbio</t>
   </si>
   <si>
     <t>Tmp 8.1</t>
@@ -900,7 +903,7 @@
     <numFmt formatCode="0.0" numFmtId="169"/>
     <numFmt formatCode="@" numFmtId="170"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -954,11 +957,6 @@
     <font>
       <name val="Arial"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
@@ -1152,7 +1150,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -1222,13 +1220,16 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="8" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="9" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="9" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
@@ -1256,16 +1257,16 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="170" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
@@ -1351,20 +1352,20 @@
   <dimension ref="A2:I45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="K35" activeCellId="2" pane="topLeft" sqref="B24:B27 B28 K35"/>
+      <selection activeCell="K35" activeCellId="0" pane="topLeft" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8039215686275"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.878431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
@@ -2023,19 +2024,19 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="B28" activeCellId="1" pane="topLeft" sqref="B24:B27 B28"/>
+      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.9176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.0196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5725490196078"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0980392156863"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
@@ -2076,7 +2077,7 @@
         <v>1.5</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -2139,23 +2140,29 @@
       <c r="G9" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="40" t="n">
-        <v>6E-010</v>
-      </c>
-      <c r="D10" s="41" t="n">
-        <v>6E-010</v>
+      <c r="C10" s="39" t="n">
+        <v>4E-008</v>
+      </c>
+      <c r="D10" s="38" t="n">
+        <v>4E-008</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="B11" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="42" t="n">
+        <v>0.001</v>
+      </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
@@ -2185,14 +2192,14 @@
       <c r="G14" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9.3" outlineLevel="0" r="15">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="42"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="43"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="30"/>
@@ -2204,27 +2211,27 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="B17" s="45" t="s">
         <v>61</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>62</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="18">
-      <c r="B18" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>64</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>65</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
@@ -2241,25 +2248,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
       <c r="B20" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="44" t="s">
         <v>71</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="21">
@@ -2267,51 +2274,51 @@
         <v>10</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="45" t="n">
+        <v>74</v>
+      </c>
+      <c r="E21" s="46" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="F21" s="46" t="n">
+      <c r="F21" s="47" t="n">
         <v>50</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="H21" s="47" t="s">
         <v>75</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="22">
       <c r="B22" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="48" t="n">
+      <c r="E22" s="49" t="n">
         <v>0.05</v>
       </c>
-      <c r="F22" s="49" t="n">
+      <c r="F22" s="50" t="n">
         <v>0.95</v>
       </c>
-      <c r="H22" s="47" t="s">
-        <v>75</v>
+      <c r="H22" s="48" t="s">
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="23">
       <c r="B23" s="30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0.8</v>
@@ -2320,24 +2327,24 @@
         <v>1.7</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="50" t="n">
+        <v>81</v>
+      </c>
+      <c r="H23" s="51" t="n">
         <v>1.3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="24">
       <c r="A24" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>100</v>
@@ -2346,27 +2353,27 @@
         <v>400</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="50" t="s">
         <v>85</v>
       </c>
+      <c r="H24" s="51" t="s">
+        <v>86</v>
+      </c>
       <c r="I24" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="25">
       <c r="A25" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>1.3</v>
@@ -2375,24 +2382,24 @@
         <v>2</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="50" t="n">
+        <v>85</v>
+      </c>
+      <c r="H25" s="51" t="n">
         <v>1.3</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="26">
       <c r="B26" s="30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -2403,25 +2410,25 @@
         <v>876</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" s="50" t="n">
+        <v>92</v>
+      </c>
+      <c r="H26" s="51" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="27">
       <c r="B27" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E27" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -2432,25 +2439,25 @@
         <v>0.019272</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="51" t="n">
+        <v>92</v>
+      </c>
+      <c r="H27" s="52" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="28">
       <c r="B28" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0.001</v>
@@ -2459,21 +2466,21 @@
         <v>10</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" s="50" t="n">
+        <v>98</v>
+      </c>
+      <c r="H28" s="51" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="29">
       <c r="A29" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="44" t="s">
         <v>99</v>
       </c>
+      <c r="B29" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="C29" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0.5</v>
@@ -2481,16 +2488,16 @@
       <c r="F29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="50" t="n">
+      <c r="H29" s="51" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="30">
-      <c r="B30" s="44" t="s">
-        <v>101</v>
+      <c r="B30" s="45" t="s">
+        <v>102</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0.5</v>
@@ -2498,77 +2505,77 @@
       <c r="F30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H30" s="50" t="n">
+      <c r="H30" s="51" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="H31" s="50"/>
+      <c r="H31" s="51"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="H32" s="50"/>
+      <c r="H32" s="51"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H33" s="50"/>
+        <v>104</v>
+      </c>
+      <c r="H33" s="51"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="47" t="n">
+        <v>108</v>
+      </c>
+      <c r="H34" s="48" t="n">
         <f aca="false">1*10^{-9}</f>
         <v>1E-009</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="52" t="n">
+      <c r="H35" s="53" t="n">
         <f aca="false">3.7*10^{-9}</f>
         <v>3.7E-009</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="45">
-      <c r="A45" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B45" s="44" t="s">
+      <c r="A45" s="45" t="s">
         <v>112</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
@@ -2605,238 +2612,238 @@
   <dimension ref="A2:AY56"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="2" pane="topLeft" sqref="B24:B27 B28 A12"/>
+      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.02352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.9254901960784"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9607843137255"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.278431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.4196078431373"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.6470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8901960784314"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.06666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.1254901960784"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.0588235294118"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.3843137254902"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.5529411764706"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
-      <c r="B2" s="53" t="s">
-        <v>113</v>
+      <c r="B2" s="54" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="J3" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K4" s="54" t="s">
         <v>119</v>
+      </c>
+      <c r="K4" s="55" t="s">
+        <v>120</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="R4" s="44" t="s">
+      <c r="Q4" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="S4" s="44"/>
+      <c r="R4" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="S4" s="45"/>
       <c r="V4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="B6" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1000</v>
@@ -2847,7 +2854,7 @@
       <c r="F6" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G6" s="55" t="n">
+      <c r="G6" s="56" t="n">
         <f aca="false">E6/J6</f>
         <v>909.090909090909</v>
       </c>
@@ -2879,36 +2886,36 @@
       <c r="P6" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q6" s="45" t="n">
+      <c r="Q6" s="46" t="n">
         <v>8E-009</v>
       </c>
-      <c r="R6" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56" t="s">
+      <c r="R6" s="57" t="s">
         <v>173</v>
       </c>
-      <c r="U6" s="56" t="s">
+      <c r="S6" s="57"/>
+      <c r="T6" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="V6" s="56" t="s">
+      <c r="U6" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="W6" s="56" t="s">
+      <c r="V6" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="X6" s="56" t="s">
+      <c r="W6" s="57" t="s">
         <v>177</v>
       </c>
+      <c r="X6" s="57" t="s">
+        <v>178</v>
+      </c>
       <c r="Y6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Z6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" s="56" t="s">
-        <v>178</v>
+      <c r="AA6" s="57" t="s">
+        <v>179</v>
       </c>
       <c r="AB6" s="0" t="n">
         <v>0</v>
@@ -2925,29 +2932,29 @@
       <c r="AF6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" s="56" t="s">
-        <v>179</v>
-      </c>
-      <c r="AH6" s="56" t="s">
+      <c r="AG6" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI6" s="56" t="s">
+      <c r="AH6" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ6" s="56" t="s">
+      <c r="AI6" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK6" s="56" t="s">
+      <c r="AJ6" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL6" s="56" t="s">
+      <c r="AK6" s="57" t="s">
         <v>184</v>
+      </c>
+      <c r="AL6" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="AM6" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN6" s="56" t="s">
-        <v>185</v>
+      <c r="AN6" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="AO6" s="0" t="n">
         <v>0</v>
@@ -2976,37 +2983,37 @@
       <c r="AW6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AX6" s="56" t="s">
-        <v>186</v>
+      <c r="AX6" s="57" t="s">
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="G7" s="55"/>
+      <c r="G7" s="56"/>
       <c r="K7" s="2"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
-      <c r="AA7" s="56"/>
-      <c r="AG7" s="56"/>
-      <c r="AH7" s="56"/>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="56"/>
-      <c r="AK7" s="56"/>
-      <c r="AL7" s="56"/>
-      <c r="AN7" s="56"/>
-      <c r="AX7" s="56"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
+      <c r="AA7" s="57"/>
+      <c r="AG7" s="57"/>
+      <c r="AH7" s="57"/>
+      <c r="AI7" s="57"/>
+      <c r="AJ7" s="57"/>
+      <c r="AK7" s="57"/>
+      <c r="AL7" s="57"/>
+      <c r="AN7" s="57"/>
+      <c r="AX7" s="57"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>500</v>
@@ -3017,7 +3024,7 @@
       <c r="F8" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="G8" s="57" t="n">
+      <c r="G8" s="58" t="n">
         <f aca="false">E8/J8</f>
         <v>374.826018814378</v>
       </c>
@@ -3027,7 +3034,7 @@
       <c r="I8" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J8" s="58" t="n">
+      <c r="J8" s="59" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D8)</f>
         <v>0.266790444047381</v>
       </c>
@@ -3050,39 +3057,39 @@
       <c r="P8" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q8" s="45" t="n">
+      <c r="Q8" s="46" t="n">
         <v>8E-009</v>
       </c>
       <c r="R8" s="2" t="n">
         <f aca="false">S8/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S8" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="T8" s="59" t="s">
+      <c r="S8" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="U8" s="59" t="s">
+      <c r="T8" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="V8" s="56" t="s">
+      <c r="U8" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="W8" s="56" t="s">
+      <c r="V8" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="X8" s="59" t="s">
+      <c r="W8" s="57" t="s">
         <v>194</v>
       </c>
+      <c r="X8" s="60" t="s">
+        <v>195</v>
+      </c>
       <c r="Y8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Z8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="56" t="s">
-        <v>178</v>
+      <c r="AA8" s="57" t="s">
+        <v>179</v>
       </c>
       <c r="AB8" s="0" t="n">
         <v>0</v>
@@ -3099,29 +3106,29 @@
       <c r="AF8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG8" s="56" t="s">
-        <v>179</v>
-      </c>
-      <c r="AH8" s="56" t="s">
+      <c r="AG8" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI8" s="56" t="s">
+      <c r="AH8" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ8" s="56" t="s">
+      <c r="AI8" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK8" s="56" t="s">
+      <c r="AJ8" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL8" s="56" t="s">
+      <c r="AK8" s="57" t="s">
         <v>184</v>
+      </c>
+      <c r="AL8" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="AM8" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN8" s="56" t="s">
-        <v>185</v>
+      <c r="AN8" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="AO8" s="0" t="n">
         <v>0</v>
@@ -3150,7 +3157,7 @@
       <c r="AW8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AX8" s="60" t="n">
+      <c r="AX8" s="61" t="n">
         <v>0.00010417</v>
       </c>
       <c r="AY8" s="0" t="n">
@@ -3159,478 +3166,478 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="54" t="n">
+        <v>197</v>
+      </c>
+      <c r="D9" s="55" t="n">
         <v>500</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="55" t="n">
         <v>100</v>
       </c>
-      <c r="F9" s="54" t="n">
+      <c r="F9" s="55" t="n">
         <v>1000</v>
       </c>
-      <c r="G9" s="61" t="n">
+      <c r="G9" s="62" t="n">
         <f aca="false">E9/J9</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H9" s="54" t="n">
+      <c r="H9" s="55" t="n">
         <v>8.1</v>
       </c>
-      <c r="I9" s="54" t="n">
+      <c r="I9" s="55" t="n">
         <v>35</v>
       </c>
-      <c r="J9" s="62" t="n">
+      <c r="J9" s="63" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D9)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K9" s="54" t="n">
+      <c r="K9" s="55" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D9))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L9" s="54" t="n">
+      <c r="L9" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="54" t="n">
+      <c r="M9" s="55" t="n">
         <v>0.85</v>
       </c>
-      <c r="N9" s="54" t="n">
+      <c r="N9" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="54" t="n">
+      <c r="O9" s="55" t="n">
         <v>0.174</v>
       </c>
-      <c r="P9" s="54" t="n">
+      <c r="P9" s="55" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q9" s="63" t="n">
+      <c r="Q9" s="64" t="n">
         <v>8E-009</v>
       </c>
       <c r="R9" s="0" t="n">
         <f aca="false">S9/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="T9" s="56" t="s">
+      <c r="S9" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="U9" s="56" t="s">
+      <c r="T9" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="V9" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="W9" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="X9" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="56" t="s">
+      <c r="U9" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="V9" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="W9" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="X9" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="AH9" s="56" t="s">
+      <c r="AB9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI9" s="56" t="s">
+      <c r="AH9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ9" s="56" t="s">
+      <c r="AI9" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK9" s="56" t="s">
+      <c r="AJ9" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL9" s="56" t="s">
+      <c r="AK9" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="AM9" s="54" t="n">
+      <c r="AL9" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM9" s="55" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN9" s="56" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="63" t="n">
+      <c r="AN9" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="64" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY9" s="54" t="n">
+      <c r="AY9" s="55" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="B10" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="54" t="n">
+        <v>200</v>
+      </c>
+      <c r="D10" s="55" t="n">
         <v>500</v>
       </c>
-      <c r="E10" s="54" t="n">
+      <c r="E10" s="55" t="n">
         <v>100</v>
       </c>
-      <c r="F10" s="54" t="n">
+      <c r="F10" s="55" t="n">
         <v>1000</v>
       </c>
-      <c r="G10" s="61" t="n">
+      <c r="G10" s="62" t="n">
         <f aca="false">E10/J10</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H10" s="54" t="n">
+      <c r="H10" s="55" t="n">
         <v>8.1</v>
       </c>
-      <c r="I10" s="54" t="n">
+      <c r="I10" s="55" t="n">
         <v>35</v>
       </c>
-      <c r="J10" s="62" t="n">
+      <c r="J10" s="63" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D10)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K10" s="54" t="n">
+      <c r="K10" s="55" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D10))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L10" s="54" t="n">
+      <c r="L10" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="M10" s="54" t="n">
+      <c r="M10" s="55" t="n">
         <v>0.85</v>
       </c>
-      <c r="N10" s="54" t="n">
+      <c r="N10" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="54" t="n">
+      <c r="O10" s="55" t="n">
         <v>0.174</v>
       </c>
-      <c r="P10" s="54" t="n">
+      <c r="P10" s="55" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q10" s="63" t="n">
+      <c r="Q10" s="64" t="n">
         <v>8E-009</v>
       </c>
       <c r="R10" s="0" t="n">
         <f aca="false">S10/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="T10" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="U10" s="59" t="s">
+      <c r="S10" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="T10" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="V10" s="56" t="s">
-        <v>192</v>
-      </c>
-      <c r="W10" s="56" t="s">
+      <c r="U10" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="V10" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="X10" s="56" t="s">
+      <c r="W10" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="Y10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="56" t="s">
+      <c r="X10" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="AH10" s="56" t="s">
+      <c r="AB10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI10" s="56" t="s">
+      <c r="AH10" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ10" s="56" t="s">
+      <c r="AI10" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK10" s="56" t="s">
+      <c r="AJ10" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL10" s="56" t="s">
+      <c r="AK10" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="AM10" s="54" t="n">
+      <c r="AL10" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM10" s="55" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN10" s="56" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="63" t="n">
+      <c r="AN10" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="64" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY10" s="54" t="n">
+      <c r="AY10" s="55" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="54" t="n">
+        <v>204</v>
+      </c>
+      <c r="D11" s="55" t="n">
         <v>500</v>
       </c>
-      <c r="E11" s="54" t="n">
+      <c r="E11" s="55" t="n">
         <v>100</v>
       </c>
-      <c r="F11" s="54" t="n">
+      <c r="F11" s="55" t="n">
         <v>1000</v>
       </c>
-      <c r="G11" s="61" t="n">
+      <c r="G11" s="62" t="n">
         <f aca="false">E11/J11</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H11" s="54" t="n">
+      <c r="H11" s="55" t="n">
         <v>8.1</v>
       </c>
-      <c r="I11" s="54" t="n">
+      <c r="I11" s="55" t="n">
         <v>35</v>
       </c>
-      <c r="J11" s="62" t="n">
+      <c r="J11" s="63" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D11)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K11" s="54" t="n">
+      <c r="K11" s="55" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D11))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L11" s="54" t="n">
+      <c r="L11" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="54" t="n">
+      <c r="M11" s="55" t="n">
         <v>0.85</v>
       </c>
-      <c r="N11" s="54" t="n">
+      <c r="N11" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="54" t="n">
+      <c r="O11" s="55" t="n">
         <v>0.174</v>
       </c>
-      <c r="P11" s="54" t="n">
+      <c r="P11" s="55" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q11" s="63" t="n">
+      <c r="Q11" s="64" t="n">
         <v>8E-009</v>
       </c>
       <c r="R11" s="0" t="n">
         <f aca="false">S11/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="T11" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="U11" s="59" t="s">
+      <c r="S11" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="T11" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="V11" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="W11" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="X11" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="56" t="s">
+      <c r="U11" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="V11" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="W11" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="X11" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="AH11" s="56" t="s">
+      <c r="AB11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI11" s="56" t="s">
+      <c r="AH11" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ11" s="56" t="s">
+      <c r="AI11" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK11" s="56" t="s">
+      <c r="AJ11" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL11" s="56" t="s">
+      <c r="AK11" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="AM11" s="54" t="n">
+      <c r="AL11" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM11" s="55" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN11" s="56" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="63" t="n">
+      <c r="AN11" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="64" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY11" s="54" t="n">
+      <c r="AY11" s="55" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="B12" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>5000</v>
@@ -3641,9 +3648,9 @@
       <c r="F12" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="G12" s="57" t="n">
+      <c r="G12" s="58" t="n">
         <f aca="false">E12/J12</f>
-        <v>34030.609703112</v>
+        <v>34030.6097031119</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.4</v>
@@ -3651,7 +3658,7 @@
       <c r="I12" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J12" s="58" t="n">
+      <c r="J12" s="59" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D12)</f>
         <v>0.00293853095411498</v>
       </c>
@@ -3674,314 +3681,314 @@
       <c r="P12" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q12" s="45" t="n">
+      <c r="Q12" s="46" t="n">
         <v>8E-009</v>
       </c>
       <c r="R12" s="2" t="n">
         <f aca="false">S12/(100*12)*2.5</f>
         <v>1.04166666666667E-005</v>
       </c>
-      <c r="S12" s="59" t="s">
-        <v>206</v>
-      </c>
-      <c r="T12" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="U12" s="56" t="s">
+      <c r="S12" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="T12" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="V12" s="56" t="s">
+      <c r="U12" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="W12" s="56" t="s">
+      <c r="V12" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="X12" s="56" t="s">
+      <c r="W12" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="Y12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="56" t="s">
+      <c r="X12" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="AH12" s="56" t="s">
+      <c r="AB12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="AI12" s="56" t="s">
+      <c r="AH12" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="AJ12" s="56" t="s">
+      <c r="AI12" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="AK12" s="56" t="s">
+      <c r="AJ12" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="AL12" s="56" t="s">
+      <c r="AK12" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="AM12" s="54" t="n">
+      <c r="AL12" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM12" s="55" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN12" s="56" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="54" t="n">
+      <c r="AN12" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="55" t="n">
         <v>0</v>
       </c>
       <c r="AX12" s="2" t="n">
         <f aca="false">AY12/(100*12)*2.5</f>
         <v>1.04166666666667E-005</v>
       </c>
-      <c r="AY12" s="59" t="s">
-        <v>206</v>
+      <c r="AY12" s="60" t="s">
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
-      <c r="B17" s="44" t="s">
-        <v>207</v>
+      <c r="B17" s="45" t="s">
+        <v>208</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="B23" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="B27" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="B29" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>221</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>220</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="B31" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="B32" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="B34" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="B37" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="B38" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="B39" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="B40" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="B41" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="B43" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="B45" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="B46" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="B47" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="B48" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="B49" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="B51" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="B52" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="B53" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="B54" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="B55" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="B56" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4003,17 +4010,17 @@
   <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B24:B27 B28"/>
+      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5960784313725"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.72941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.321568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.8313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.4588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -4021,113 +4028,113 @@
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>244</v>
-      </c>
-      <c r="I3" s="65"/>
+        <v>71</v>
+      </c>
+      <c r="H3" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="I3" s="66"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="46" t="n">
+        <v>74</v>
+      </c>
+      <c r="E4" s="47" t="n">
         <v>6E-007</v>
       </c>
-      <c r="F4" s="46" t="n">
+      <c r="F4" s="47" t="n">
         <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="66" t="n">
+        <v>75</v>
+      </c>
+      <c r="H4" s="67" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="I4" s="65" t="n">
+      <c r="I4" s="66" t="n">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="B5" s="30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="46" t="n">
+        <v>74</v>
+      </c>
+      <c r="E5" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="47" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="66" t="n">
+        <v>75</v>
+      </c>
+      <c r="H5" s="67" t="n">
         <f aca="false">1*10^{-6}</f>
         <v>1E-006</v>
       </c>
-      <c r="I5" s="66" t="n">
+      <c r="I5" s="67" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="6">
       <c r="B6" s="30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="7">
       <c r="A7" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>250</v>
@@ -4136,16 +4143,16 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="30"/>
       <c r="D8" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>108</v>
@@ -4154,21 +4161,21 @@
         <v>243</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="9">
       <c r="A9" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1.3</v>
@@ -4177,30 +4184,30 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="30"/>
       <c r="D10" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="B11" s="30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -4211,25 +4218,25 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="B12" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -4240,25 +4247,25 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="67" t="n">
+        <v>92</v>
+      </c>
+      <c r="H12" s="68" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">1*10^{-6}*24*365</f>
@@ -4269,25 +4276,25 @@
         <v>4.38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="54" t="n">
+        <v>92</v>
+      </c>
+      <c r="H13" s="55" t="n">
         <f aca="false">365*1*10^{-3}</f>
         <v>0.365</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="B14" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.001</v>
@@ -4296,40 +4303,40 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
       <c r="A17" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="44" t="s">
         <v>99</v>
       </c>
+      <c r="B17" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="C17" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.5</v>
@@ -4339,11 +4346,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="18">
-      <c r="B18" s="44" t="s">
-        <v>101</v>
+      <c r="B18" s="45" t="s">
+        <v>102</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.5</v>
@@ -4354,7 +4361,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added OMEN-workflow PAWN & created figures
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="492" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="328" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="SWI fluxes comparison" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,6 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
-            <charset val="1"/>
             <family val="2"/>
             <b val="true"/>
             <color rgb="00000000"/>
@@ -40,7 +39,6 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
-            <charset val="1"/>
             <family val="2"/>
             <color rgb="00000000"/>
             <sz val="9"/>
@@ -299,7 +297,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -324,7 +321,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -335,7 +331,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -363,7 +358,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -374,7 +368,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -423,7 +416,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -442,7 +434,6 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -906,7 +897,6 @@
   <fonts count="16">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -927,14 +917,12 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -942,27 +930,23 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <color rgb="00FF0000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -970,7 +954,6 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -978,14 +961,12 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -993,13 +974,11 @@
     </font>
     <font>
       <name val="arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Verdana"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00000000"/>
@@ -1007,7 +986,6 @@
     </font>
     <font>
       <name val="Verdana"/>
-      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="9"/>
@@ -1356,16 +1334,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6392156862745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.878431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2352941176471"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
@@ -2024,19 +2002,19 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0980392156863"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7294117647059"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.2823529411765"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
@@ -2060,10 +2038,10 @@
         <v>55</v>
       </c>
       <c r="C4" s="35" t="n">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="D4" s="36" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
@@ -2616,26 +2594,26 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3176470588235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.06666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.1254901960784"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2235294117647"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.0588235294118"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2235294117647"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.3843137254902"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.5529411764706"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4862745098039"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.956862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.3333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.3137254901961"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1607843137255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.3137254901961"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.4862745098039"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.6823529411765"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.0823529411765"/>
+    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -3650,7 +3628,7 @@
       </c>
       <c r="G12" s="58" t="n">
         <f aca="false">E12/J12</f>
-        <v>34030.6097031119</v>
+        <v>34030.609703112</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.4</v>
@@ -4014,13 +3992,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.8313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.77254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.4588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.356862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.5960784313725"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">

</xml_diff>

<commit_message>
added profiles and SA plots
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -28,6 +28,7 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
+            <charset val="1"/>
             <family val="2"/>
             <b val="true"/>
             <color rgb="00000000"/>
@@ -39,6 +40,7 @@
         <r>
           <rPr>
             <rFont val="Verdana"/>
+            <charset val="1"/>
             <family val="2"/>
             <color rgb="00000000"/>
             <sz val="9"/>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="252">
   <si>
     <t>Thullner et al. 2009</t>
   </si>
@@ -232,6 +234,15 @@
   </si>
   <si>
     <t>zbio</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>tort</t>
+  </si>
+  <si>
+    <t>irrigFact</t>
   </si>
   <si>
     <t>Tmp 8.1</t>
@@ -297,6 +308,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -321,6 +333,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -331,6 +344,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -358,6 +372,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -368,6 +383,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -416,6 +432,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -434,6 +451,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="true"/>
         <sz val="12"/>
@@ -897,6 +915,7 @@
   <fonts count="16">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -917,12 +936,14 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -930,23 +951,27 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00FF0000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -954,6 +979,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
@@ -961,12 +987,14 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FF0000"/>
@@ -974,11 +1002,13 @@
     </font>
     <font>
       <name val="arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Verdana"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00000000"/>
@@ -986,6 +1016,7 @@
     </font>
     <font>
       <name val="Verdana"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="9"/>
@@ -1128,7 +1159,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -1199,6 +1230,9 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
@@ -1334,16 +1368,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3960784313725"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3960784313725"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
@@ -1999,22 +2033,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.2823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.2117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
@@ -2132,13 +2166,13 @@
       <c r="G10" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="41" t="n">
+      <c r="C11" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="42" t="n">
+      <c r="D11" s="36" t="n">
         <v>0.001</v>
       </c>
       <c r="E11" s="30"/>
@@ -2146,38 +2180,60 @@
       <c r="G11" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="B12" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="35" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="D12" s="36" t="n">
+        <v>2.6</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="B13" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="35" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="36" t="n">
+        <v>0.85</v>
+      </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="B14" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="36" t="n">
+        <v>3</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9.3" outlineLevel="0" r="15">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="43"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
+      <c r="B15" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="30"/>
@@ -2188,33 +2244,19 @@
       <c r="G16" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="18">
-      <c r="B18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9.3" outlineLevel="0" r="18">
+      <c r="A18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="44"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="B19" s="30"/>
@@ -2225,349 +2267,386 @@
       <c r="G19" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
-      <c r="B20" s="30" t="s">
+      <c r="A20" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="21">
+      <c r="B21" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="C21" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="22">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="23">
+      <c r="B23" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="C23" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="D23" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="E23" s="30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="21">
-      <c r="B21" s="30" t="s">
+      <c r="F23" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="24">
+      <c r="B24" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="46" t="n">
+      <c r="C24" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="47" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="F21" s="47" t="n">
+      <c r="F24" s="48" t="n">
         <v>50</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="22">
-      <c r="B22" s="30" t="s">
+      <c r="G24" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="25">
+      <c r="B25" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="50" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F25" s="51" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="26">
+      <c r="B26" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="52" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="27">
+      <c r="A27" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="28">
+      <c r="A28" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="52" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="29">
+      <c r="B29" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="49" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F22" s="50" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="23">
-      <c r="B23" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="51" t="n">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="24">
-      <c r="A24" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="25">
-      <c r="A25" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25" s="51" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="26">
-      <c r="B26" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="0" t="n">
+      <c r="E29" s="0" t="n">
         <f aca="false">0.005*24*365</f>
         <v>43.8</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F29" s="0" t="n">
         <f aca="false">0.1*24*365</f>
         <v>876</v>
       </c>
-      <c r="G26" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" s="51" t="n">
+      <c r="G29" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="52" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="27">
-      <c r="B27" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="0" t="n">
+      <c r="I29" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="30">
+      <c r="B30" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
         <v>0.015768</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F30" s="0" t="n">
         <f aca="false">2.2*10^{-6}*24*365</f>
         <v>0.019272</v>
       </c>
-      <c r="G27" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="52" t="n">
+      <c r="G30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="53" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="28">
-      <c r="B28" s="30" t="s">
+      <c r="I30" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="0" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="31">
+      <c r="B31" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F31" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="51" t="n">
+      <c r="G31" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" s="52" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="29">
-      <c r="A29" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="32">
+      <c r="A32" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F32" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="51" t="n">
+      <c r="H32" s="52" t="n">
         <v>0.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="30">
-      <c r="B30" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="33">
+      <c r="B33" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H30" s="51" t="n">
+      <c r="H33" s="52" t="n">
         <v>0.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="H31" s="51"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="H32" s="51"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="B33" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H33" s="51"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="34">
-      <c r="A34" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="H34" s="52"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="H35" s="52"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="B36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="H36" s="52"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="48" t="n">
+      <c r="B37" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" s="49" t="n">
         <f aca="false">1*10^{-9}</f>
         <v>1E-009</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="35">
-      <c r="A35" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="I37" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="53" t="n">
+      <c r="B38" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="54" t="n">
         <f aca="false">3.7*10^{-9}</f>
         <v>3.7E-009</v>
       </c>
-      <c r="I35" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="C38" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="45">
-      <c r="A45" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
-      <c r="B46" s="0" t="n">
+      <c r="I38" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="C41" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="48">
+      <c r="A48" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="B49" s="0" t="n">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
-      <c r="B47" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="B50" s="0" t="n">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
-      <c r="B48" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="B51" s="0" t="n">
         <v>164</v>
       </c>
     </row>
@@ -2594,234 +2673,234 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.956862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.3333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1607843137255"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.4862745098039"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.6823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.0823529411765"/>
-    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.7529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0274509803922"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.14117647058824"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.5411764705882"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.2666666666667"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.5843137254902"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.8156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1372549019608"/>
+    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
-      <c r="B2" s="54" t="s">
-        <v>114</v>
+      <c r="B2" s="55" t="s">
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="J3" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" s="55" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="K4" s="56" t="s">
+        <v>123</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="R4" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="S4" s="45"/>
+      <c r="Q4" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="S4" s="46"/>
       <c r="V4" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="B6" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1000</v>
@@ -2832,7 +2911,7 @@
       <c r="F6" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G6" s="56" t="n">
+      <c r="G6" s="57" t="n">
         <f aca="false">E6/J6</f>
         <v>909.090909090909</v>
       </c>
@@ -2864,36 +2943,36 @@
       <c r="P6" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q6" s="46" t="n">
+      <c r="Q6" s="47" t="n">
         <v>8E-009</v>
       </c>
-      <c r="R6" s="57" t="s">
-        <v>173</v>
-      </c>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57" t="s">
-        <v>174</v>
-      </c>
-      <c r="U6" s="57" t="s">
-        <v>175</v>
-      </c>
-      <c r="V6" s="57" t="s">
+      <c r="R6" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="W6" s="57" t="s">
+      <c r="S6" s="58"/>
+      <c r="T6" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="X6" s="57" t="s">
+      <c r="U6" s="58" t="s">
         <v>178</v>
       </c>
+      <c r="V6" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="W6" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="X6" s="58" t="s">
+        <v>181</v>
+      </c>
       <c r="Y6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Z6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" s="57" t="s">
-        <v>179</v>
+      <c r="AA6" s="58" t="s">
+        <v>182</v>
       </c>
       <c r="AB6" s="0" t="n">
         <v>0</v>
@@ -2910,29 +2989,29 @@
       <c r="AF6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH6" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI6" s="57" t="s">
-        <v>182</v>
-      </c>
-      <c r="AJ6" s="57" t="s">
+      <c r="AG6" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK6" s="57" t="s">
+      <c r="AH6" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL6" s="57" t="s">
+      <c r="AI6" s="58" t="s">
         <v>185</v>
+      </c>
+      <c r="AJ6" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK6" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL6" s="58" t="s">
+        <v>188</v>
       </c>
       <c r="AM6" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN6" s="57" t="s">
-        <v>186</v>
+      <c r="AN6" s="58" t="s">
+        <v>189</v>
       </c>
       <c r="AO6" s="0" t="n">
         <v>0</v>
@@ -2961,37 +3040,37 @@
       <c r="AW6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AX6" s="57" t="s">
-        <v>187</v>
+      <c r="AX6" s="58" t="s">
+        <v>190</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="G7" s="56"/>
+      <c r="G7" s="57"/>
       <c r="K7" s="2"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="AA7" s="57"/>
-      <c r="AG7" s="57"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="57"/>
-      <c r="AJ7" s="57"/>
-      <c r="AK7" s="57"/>
-      <c r="AL7" s="57"/>
-      <c r="AN7" s="57"/>
-      <c r="AX7" s="57"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="58"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="58"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AX7" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>500</v>
@@ -3002,7 +3081,7 @@
       <c r="F8" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="G8" s="58" t="n">
+      <c r="G8" s="59" t="n">
         <f aca="false">E8/J8</f>
         <v>374.826018814378</v>
       </c>
@@ -3012,7 +3091,7 @@
       <c r="I8" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J8" s="59" t="n">
+      <c r="J8" s="60" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D8)</f>
         <v>0.266790444047381</v>
       </c>
@@ -3035,39 +3114,39 @@
       <c r="P8" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q8" s="46" t="n">
+      <c r="Q8" s="47" t="n">
         <v>8E-009</v>
       </c>
       <c r="R8" s="2" t="n">
         <f aca="false">S8/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S8" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="T8" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="U8" s="60" t="s">
-        <v>192</v>
-      </c>
-      <c r="V8" s="57" t="s">
+      <c r="S8" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="W8" s="57" t="s">
+      <c r="T8" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="X8" s="60" t="s">
+      <c r="U8" s="61" t="s">
         <v>195</v>
       </c>
+      <c r="V8" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="W8" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="X8" s="61" t="s">
+        <v>198</v>
+      </c>
       <c r="Y8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="Z8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="57" t="s">
-        <v>179</v>
+      <c r="AA8" s="58" t="s">
+        <v>182</v>
       </c>
       <c r="AB8" s="0" t="n">
         <v>0</v>
@@ -3084,29 +3163,29 @@
       <c r="AF8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AG8" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH8" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI8" s="57" t="s">
-        <v>182</v>
-      </c>
-      <c r="AJ8" s="57" t="s">
+      <c r="AG8" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK8" s="57" t="s">
+      <c r="AH8" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL8" s="57" t="s">
+      <c r="AI8" s="58" t="s">
         <v>185</v>
+      </c>
+      <c r="AJ8" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK8" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL8" s="58" t="s">
+        <v>188</v>
       </c>
       <c r="AM8" s="0" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN8" s="57" t="s">
-        <v>186</v>
+      <c r="AN8" s="58" t="s">
+        <v>189</v>
       </c>
       <c r="AO8" s="0" t="n">
         <v>0</v>
@@ -3135,7 +3214,7 @@
       <c r="AW8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AX8" s="61" t="n">
+      <c r="AX8" s="62" t="n">
         <v>0.00010417</v>
       </c>
       <c r="AY8" s="0" t="n">
@@ -3144,478 +3223,478 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="B9" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="55" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" s="56" t="n">
         <v>500</v>
       </c>
-      <c r="E9" s="55" t="n">
+      <c r="E9" s="56" t="n">
         <v>100</v>
       </c>
-      <c r="F9" s="55" t="n">
+      <c r="F9" s="56" t="n">
         <v>1000</v>
       </c>
-      <c r="G9" s="62" t="n">
+      <c r="G9" s="63" t="n">
         <f aca="false">E9/J9</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H9" s="55" t="n">
+      <c r="H9" s="56" t="n">
         <v>8.1</v>
       </c>
-      <c r="I9" s="55" t="n">
+      <c r="I9" s="56" t="n">
         <v>35</v>
       </c>
-      <c r="J9" s="63" t="n">
+      <c r="J9" s="64" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D9)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K9" s="55" t="n">
+      <c r="K9" s="56" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D9))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L9" s="55" t="n">
+      <c r="L9" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="55" t="n">
+      <c r="M9" s="56" t="n">
         <v>0.85</v>
       </c>
-      <c r="N9" s="55" t="n">
+      <c r="N9" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="55" t="n">
+      <c r="O9" s="56" t="n">
         <v>0.174</v>
       </c>
-      <c r="P9" s="55" t="n">
+      <c r="P9" s="56" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q9" s="64" t="n">
+      <c r="Q9" s="65" t="n">
         <v>8E-009</v>
       </c>
       <c r="R9" s="0" t="n">
         <f aca="false">S9/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S9" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="T9" s="57" t="s">
-        <v>191</v>
-      </c>
-      <c r="U9" s="57" t="s">
-        <v>192</v>
-      </c>
-      <c r="V9" s="60" t="s">
+      <c r="S9" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="T9" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="U9" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="V9" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="W9" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="X9" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="W9" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="X9" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="Y9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH9" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI9" s="57" t="s">
+      <c r="Y9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="AJ9" s="57" t="s">
+      <c r="AB9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK9" s="57" t="s">
+      <c r="AH9" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL9" s="57" t="s">
+      <c r="AI9" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="AM9" s="55" t="n">
+      <c r="AJ9" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK9" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL9" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM9" s="56" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN9" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="64" t="n">
+      <c r="AN9" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="65" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY9" s="55" t="n">
+      <c r="AY9" s="56" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="B10" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="D10" s="55" t="n">
+        <v>203</v>
+      </c>
+      <c r="D10" s="56" t="n">
         <v>500</v>
       </c>
-      <c r="E10" s="55" t="n">
+      <c r="E10" s="56" t="n">
         <v>100</v>
       </c>
-      <c r="F10" s="55" t="n">
+      <c r="F10" s="56" t="n">
         <v>1000</v>
       </c>
-      <c r="G10" s="62" t="n">
+      <c r="G10" s="63" t="n">
         <f aca="false">E10/J10</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H10" s="55" t="n">
+      <c r="H10" s="56" t="n">
         <v>8.1</v>
       </c>
-      <c r="I10" s="55" t="n">
+      <c r="I10" s="56" t="n">
         <v>35</v>
       </c>
-      <c r="J10" s="63" t="n">
+      <c r="J10" s="64" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D10)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K10" s="55" t="n">
+      <c r="K10" s="56" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D10))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L10" s="55" t="n">
+      <c r="L10" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="M10" s="55" t="n">
+      <c r="M10" s="56" t="n">
         <v>0.85</v>
       </c>
-      <c r="N10" s="55" t="n">
+      <c r="N10" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="55" t="n">
+      <c r="O10" s="56" t="n">
         <v>0.174</v>
       </c>
-      <c r="P10" s="55" t="n">
+      <c r="P10" s="56" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q10" s="64" t="n">
+      <c r="Q10" s="65" t="n">
         <v>8E-009</v>
       </c>
       <c r="R10" s="0" t="n">
         <f aca="false">S10/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S10" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="T10" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="U10" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="V10" s="57" t="s">
+      <c r="S10" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="W10" s="57" t="s">
-        <v>194</v>
-      </c>
-      <c r="X10" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="Y10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH10" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI10" s="57" t="s">
+      <c r="T10" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="U10" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="V10" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="W10" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="X10" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="AJ10" s="57" t="s">
+      <c r="AB10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK10" s="57" t="s">
+      <c r="AH10" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL10" s="57" t="s">
+      <c r="AI10" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="AM10" s="55" t="n">
+      <c r="AJ10" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK10" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL10" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM10" s="56" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN10" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="64" t="n">
+      <c r="AN10" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="65" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY10" s="55" t="n">
+      <c r="AY10" s="56" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="55" t="n">
+        <v>207</v>
+      </c>
+      <c r="D11" s="56" t="n">
         <v>500</v>
       </c>
-      <c r="E11" s="55" t="n">
+      <c r="E11" s="56" t="n">
         <v>100</v>
       </c>
-      <c r="F11" s="55" t="n">
+      <c r="F11" s="56" t="n">
         <v>1000</v>
       </c>
-      <c r="G11" s="62" t="n">
+      <c r="G11" s="63" t="n">
         <f aca="false">E11/J11</f>
         <v>374.826018814378</v>
       </c>
-      <c r="H11" s="55" t="n">
+      <c r="H11" s="56" t="n">
         <v>8.1</v>
       </c>
-      <c r="I11" s="55" t="n">
+      <c r="I11" s="56" t="n">
         <v>35</v>
       </c>
-      <c r="J11" s="63" t="n">
+      <c r="J11" s="64" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D11)</f>
         <v>0.266790444047381</v>
       </c>
-      <c r="K11" s="55" t="n">
+      <c r="K11" s="56" t="n">
         <f aca="false">5.2*(10^(0.7624-0.0003972*D11))</f>
         <v>19.0459808634568</v>
       </c>
-      <c r="L11" s="55" t="n">
+      <c r="L11" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="55" t="n">
+      <c r="M11" s="56" t="n">
         <v>0.85</v>
       </c>
-      <c r="N11" s="55" t="n">
+      <c r="N11" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="55" t="n">
+      <c r="O11" s="56" t="n">
         <v>0.174</v>
       </c>
-      <c r="P11" s="55" t="n">
+      <c r="P11" s="56" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q11" s="64" t="n">
+      <c r="Q11" s="65" t="n">
         <v>8E-009</v>
       </c>
       <c r="R11" s="0" t="n">
         <f aca="false">S11/(100*12)*2.5</f>
         <v>0.000104166666666667</v>
       </c>
-      <c r="S11" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="T11" s="60" t="s">
+      <c r="S11" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="T11" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="U11" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="V11" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="U11" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="V11" s="60" t="s">
+      <c r="W11" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="X11" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="W11" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="X11" s="57" t="s">
-        <v>195</v>
-      </c>
-      <c r="Y11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH11" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI11" s="57" t="s">
+      <c r="Y11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="AJ11" s="57" t="s">
+      <c r="AB11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK11" s="57" t="s">
+      <c r="AH11" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL11" s="57" t="s">
+      <c r="AI11" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="AM11" s="55" t="n">
+      <c r="AJ11" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK11" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL11" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM11" s="56" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN11" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="64" t="n">
+      <c r="AN11" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="65" t="n">
         <v>0.00010417</v>
       </c>
-      <c r="AY11" s="55" t="n">
+      <c r="AY11" s="56" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="B12" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>5000</v>
@@ -3626,9 +3705,9 @@
       <c r="F12" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="G12" s="58" t="n">
+      <c r="G12" s="59" t="n">
         <f aca="false">E12/J12</f>
-        <v>34030.609703112</v>
+        <v>34030.6097031119</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.4</v>
@@ -3636,7 +3715,7 @@
       <c r="I12" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J12" s="59" t="n">
+      <c r="J12" s="60" t="n">
         <f aca="false">3.3*10^(-0.87478367-0.00043512*D12)</f>
         <v>0.00293853095411498</v>
       </c>
@@ -3659,314 +3738,314 @@
       <c r="P12" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q12" s="46" t="n">
+      <c r="Q12" s="47" t="n">
         <v>8E-009</v>
       </c>
       <c r="R12" s="2" t="n">
         <f aca="false">S12/(100*12)*2.5</f>
         <v>1.04166666666667E-005</v>
       </c>
-      <c r="S12" s="60" t="s">
-        <v>207</v>
-      </c>
-      <c r="T12" s="57" t="s">
-        <v>191</v>
-      </c>
-      <c r="U12" s="57" t="s">
-        <v>192</v>
-      </c>
-      <c r="V12" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="W12" s="57" t="s">
+      <c r="S12" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="T12" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="X12" s="57" t="s">
+      <c r="U12" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="Y12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH12" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI12" s="57" t="s">
+      <c r="V12" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="W12" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="X12" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="AJ12" s="57" t="s">
+      <c r="AB12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="AK12" s="57" t="s">
+      <c r="AH12" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="AL12" s="57" t="s">
+      <c r="AI12" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="AM12" s="55" t="n">
+      <c r="AJ12" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK12" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL12" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM12" s="56" t="n">
         <v>0.35</v>
       </c>
-      <c r="AN12" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="55" t="n">
+      <c r="AN12" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="56" t="n">
         <v>0</v>
       </c>
       <c r="AX12" s="2" t="n">
         <f aca="false">AY12/(100*12)*2.5</f>
         <v>1.04166666666667E-005</v>
       </c>
-      <c r="AY12" s="60" t="s">
-        <v>207</v>
+      <c r="AY12" s="61" t="s">
+        <v>210</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
-      <c r="B17" s="45" t="s">
-        <v>208</v>
+      <c r="B17" s="46" t="s">
+        <v>211</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="B23" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="B24" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="B25" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="B26" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="B27" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="B29" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="B31" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="B32" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>224</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="B33" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="B34" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="B37" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="B38" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="B39" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="B40" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="B41" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="B43" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="B45" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="B46" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="B47" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="B48" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="B49" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="B51" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="B52" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="B53" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="B54" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="B55" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="B56" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3988,17 +4067,17 @@
   <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
+      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.356862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.0666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.5960784313725"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.3019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
@@ -4006,113 +4085,113 @@
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="65" t="s">
-        <v>245</v>
-      </c>
-      <c r="I3" s="66"/>
+        <v>74</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3" s="67"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="47" t="n">
+        <v>77</v>
+      </c>
+      <c r="E4" s="48" t="n">
         <v>6E-007</v>
       </c>
-      <c r="F4" s="47" t="n">
+      <c r="F4" s="48" t="n">
         <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="67" t="n">
+        <v>78</v>
+      </c>
+      <c r="H4" s="68" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
-      <c r="I4" s="66" t="n">
+      <c r="I4" s="67" t="n">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="B5" s="30" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="47" t="n">
+        <v>77</v>
+      </c>
+      <c r="E5" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="48" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="67" t="n">
+        <v>78</v>
+      </c>
+      <c r="H5" s="68" t="n">
         <f aca="false">1*10^{-6}</f>
         <v>1E-006</v>
       </c>
-      <c r="I5" s="67" t="n">
+      <c r="I5" s="68" t="n">
         <f aca="false">1*10^{-3}</f>
         <v>0.001</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="6">
       <c r="B6" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="7">
       <c r="A7" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>250</v>
@@ -4121,16 +4200,16 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B8" s="30"/>
       <c r="D8" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>108</v>
@@ -4139,21 +4218,21 @@
         <v>243</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="9">
       <c r="A9" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1.3</v>
@@ -4162,30 +4241,30 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B10" s="30"/>
       <c r="D10" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="B11" s="30" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">0.005*24*365</f>
@@ -4196,25 +4275,25 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="B12" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">1.8*10^{-6}*24*365</f>
@@ -4225,25 +4304,25 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="68" t="n">
+        <v>95</v>
+      </c>
+      <c r="H12" s="69" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="B13" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">1*10^{-6}*24*365</f>
@@ -4254,25 +4333,25 @@
         <v>4.38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="55" t="n">
+        <v>95</v>
+      </c>
+      <c r="H13" s="56" t="n">
         <f aca="false">365*1*10^{-3}</f>
         <v>0.365</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="B14" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>0.001</v>
@@ -4281,40 +4360,40 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="B15" s="30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="B16" s="30" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
       <c r="A17" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.5</v>
@@ -4324,11 +4403,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="18">
-      <c r="B18" s="45" t="s">
-        <v>102</v>
+      <c r="B18" s="46" t="s">
+        <v>105</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.5</v>
@@ -4339,7 +4418,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LaTex: worked on SA subsection
</commit_message>
<xml_diff>
--- a/1_Dominik_Experiments_Boundary-Conditions.xlsx
+++ b/1_Dominik_Experiments_Boundary-Conditions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="328" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="328" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SWI fluxes comparison" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,27 +23,27 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">S A:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Verdana"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">4-8 10^7</t>
         </r>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
   <si>
     <t>Thullner et al. 2009</t>
   </si>
@@ -307,12 +307,12 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="subscript"/>
       </rPr>
       <t xml:space="preserve">NH4</t>
     </r>
@@ -332,23 +332,23 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="superscript"/>
       </rPr>
       <t xml:space="preserve">I</t>
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="subscript"/>
       </rPr>
       <t xml:space="preserve">PO4</t>
     </r>
@@ -357,7 +357,7 @@
     <t>P adsorption coeff. oxic</t>
   </si>
   <si>
-    <t>Krom and Berner 1988 / Slomp et al. 1996</t>
+    <t>Krom and Berner 1988 / Slomp et al. 1998</t>
   </si>
   <si>
     <t>10 now 200</t>
@@ -371,29 +371,32 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="superscript"/>
       </rPr>
       <t xml:space="preserve">II</t>
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="subscript"/>
       </rPr>
       <t xml:space="preserve">PO4</t>
     </r>
   </si>
   <si>
     <t>P adsorption coeff. anoxic</t>
+  </si>
+  <si>
+    <t>Krom and Berner 1988 / Slomp et al. 1996</t>
   </si>
   <si>
     <t>ksPO4</t>
@@ -431,12 +434,12 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="subscript"/>
       </rPr>
       <t xml:space="preserve">NH4</t>
     </r>
@@ -450,12 +453,12 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <b val="true"/>
-        <sz val="12"/>
-        <vertAlign val="subscript"/>
       </rPr>
       <t xml:space="preserve">H2S</t>
     </r>
@@ -904,122 +907,122 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.000" numFmtId="165"/>
-    <numFmt formatCode="0.00E+000" numFmtId="166"/>
-    <numFmt formatCode="0.00E+00" numFmtId="167"/>
-    <numFmt formatCode="0.00" numFmtId="168"/>
-    <numFmt formatCode="0.0" numFmtId="169"/>
-    <numFmt formatCode="@" numFmtId="170"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00E+000"/>
+    <numFmt numFmtId="167" formatCode="0.00E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="@"/>
   </numFmts>
   <fonts count="16">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FF0000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00FF0000"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b val="true"/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
-      <vertAlign val="subscript"/>
     </font>
     <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
-      <vertAlign val="superscript"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FF0000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1031,102 +1034,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00000000"/>
-        <bgColor rgb="00003300"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00993300"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000AE00"/>
-        <bgColor rgb="00339966"/>
+        <fgColor rgb="FF00AE00"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right style="hair"/>
       <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
       <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1135,222 +1138,378 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="70">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="170" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="0000AE00"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF00AE00"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1363,24 +1522,25 @@
   </sheetPr>
   <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="K35" activeCellId="0" pane="topLeft" sqref="K35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3960784313725"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0235294117647"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3960784313725"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.8061224489796"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
@@ -1396,12 +1556,12 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
@@ -1409,8 +1569,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1431,7 +1591,7 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1616,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1477,7 +1637,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +1658,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1679,7 @@
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1540,7 +1700,7 @@
       </c>
       <c r="I14" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1721,7 @@
       </c>
       <c r="I15" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1742,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1603,7 +1763,7 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1624,7 +1784,7 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1809,7 @@
       </c>
       <c r="I19" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1674,7 +1834,7 @@
       </c>
       <c r="I20" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +1855,7 @@
       </c>
       <c r="I21" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -1706,7 +1866,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.25" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
@@ -1762,7 +1922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.85" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="24.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
@@ -1787,7 +1947,7 @@
       </c>
       <c r="I25" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
@@ -1808,7 +1968,7 @@
       </c>
       <c r="I26" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -1819,7 +1979,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
         <v>36</v>
       </c>
@@ -1832,7 +1992,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>12</v>
       </c>
@@ -1853,7 +2013,7 @@
       </c>
       <c r="I29" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
         <v>13</v>
       </c>
@@ -1874,7 +2034,7 @@
       </c>
       <c r="I30" s="8"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
         <v>14</v>
       </c>
@@ -1895,7 +2055,7 @@
       </c>
       <c r="I31" s="21"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
         <v>37</v>
       </c>
@@ -1903,19 +2063,19 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1931,7 +2091,7 @@
       </c>
       <c r="G38" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="7" t="s">
         <v>45</v>
       </c>
@@ -1944,7 +2104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="7" t="s">
         <v>48</v>
       </c>
@@ -1960,7 +2120,7 @@
         <v>1E-006</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="26" t="s">
         <v>50</v>
       </c>
@@ -1976,7 +2136,7 @@
         <v>2E-006</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row r="42" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E42" s="7"/>
       <c r="F42" s="0" t="n">
         <v>50</v>
@@ -1986,7 +2146,7 @@
         <v>5E-006</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E43" s="7"/>
       <c r="F43" s="0" t="n">
         <v>100</v>
@@ -1996,7 +2156,7 @@
         <v>1E-005</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row r="44" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E44" s="7"/>
       <c r="F44" s="28" t="n">
         <v>160</v>
@@ -2006,7 +2166,7 @@
         <v>1.6E-005</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row r="45" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E45" s="26" t="s">
         <v>52</v>
       </c>
@@ -2020,7 +2180,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2035,28 +2195,29 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5372549019608"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.2117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4705882352941"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.219387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.8826530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86224489795918"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
         <v>53</v>
@@ -2067,7 +2228,7 @@
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="34" t="s">
         <v>55</v>
       </c>
@@ -2081,7 +2242,7 @@
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="34" t="s">
         <v>56</v>
       </c>
@@ -2095,7 +2256,7 @@
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="34" t="s">
         <v>57</v>
       </c>
@@ -2109,7 +2270,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="34" t="s">
         <v>12</v>
       </c>
@@ -2123,7 +2284,7 @@
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="34" t="s">
         <v>13</v>
       </c>
@@ -2137,7 +2298,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="34" t="s">
         <v>14</v>
       </c>
@@ -2151,7 +2312,7 @@
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="34" t="s">
         <v>58</v>
       </c>
@@ -2165,7 +2326,7 @@
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="34" t="s">
         <v>59</v>
       </c>
@@ -2179,7 +2340,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="34" t="s">
         <v>60</v>
       </c>
@@ -2193,7 +2354,7 @@
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="34" t="s">
         <v>8</v>
       </c>
@@ -2207,7 +2368,7 @@
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="34" t="s">
         <v>61</v>
       </c>
@@ -2221,7 +2382,7 @@
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="41" t="s">
         <v>62</v>
       </c>
@@ -2235,7 +2396,7 @@
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -2243,12 +2404,12 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9.3" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="44"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
@@ -2258,7 +2419,7 @@
       <c r="G18" s="45"/>
       <c r="H18" s="44"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -2266,7 +2427,7 @@
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
@@ -2283,7 +2444,7 @@
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="46" t="s">
         <v>67</v>
       </c>
@@ -2295,7 +2456,7 @@
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -2303,7 +2464,7 @@
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="30" t="s">
         <v>69</v>
       </c>
@@ -2326,7 +2487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
         <v>10</v>
       </c>
@@ -2350,7 +2511,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
         <v>80</v>
       </c>
@@ -2370,7 +2531,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
         <v>82</v>
       </c>
@@ -2390,7 +2551,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
         <v>85</v>
       </c>
@@ -2419,7 +2580,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
         <v>85</v>
       </c>
@@ -2439,7 +2600,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H28" s="52" t="n">
         <v>1.3</v>
@@ -2448,12 +2609,12 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>77</v>
@@ -2467,22 +2628,22 @@
         <v>876</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H29" s="52" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="30">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>77</v>
@@ -2496,22 +2657,22 @@
         <v>0.019272</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H30" s="53" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="31">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>77</v>
@@ -2523,21 +2684,21 @@
         <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H31" s="52" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0.5</v>
@@ -2549,12 +2710,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.9" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>0.5</v>
@@ -2566,86 +2727,86 @@
         <v>0.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H34" s="52"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H35" s="52"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H36" s="52"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="37">
+    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H37" s="49" t="n">
         <f aca="false">1*10^{-9}</f>
         <v>1E-009</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="38">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B38" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>111</v>
       </c>
       <c r="H38" s="54" t="n">
         <f aca="false">3.7*10^{-9}</f>
         <v>3.7E-009</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="48">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
+    <row r="50" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
+    <row r="51" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>164</v>
       </c>
@@ -2653,7 +2814,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2668,63 +2829,64 @@
   </sheetPr>
   <dimension ref="A2:AY56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4509803921569"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0274509803922"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.14117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.5411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.2666666666667"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.5843137254902"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.8156862745098"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1372549019608"/>
-    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4540816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.14285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.5408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4030612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.5918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.8163265306122"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1377551020408"/>
+    <col collapsed="false" hidden="false" max="49" min="19" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.86224489795918"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="55" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J3" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K4" s="56" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2732,175 +2894,175 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R4" s="46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="S4" s="46"/>
       <c r="V4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AX4" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1000</v>
@@ -2947,23 +3109,23 @@
         <v>8E-009</v>
       </c>
       <c r="R6" s="58" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="S6" s="58"/>
       <c r="T6" s="58" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="U6" s="58" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="V6" s="58" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="W6" s="58" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="X6" s="58" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Y6" s="0" t="n">
         <v>0</v>
@@ -2972,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB6" s="0" t="n">
         <v>0</v>
@@ -2990,28 +3152,28 @@
         <v>0</v>
       </c>
       <c r="AG6" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH6" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI6" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ6" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK6" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL6" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM6" s="0" t="n">
         <v>0.35</v>
       </c>
       <c r="AN6" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO6" s="0" t="n">
         <v>0</v>
@@ -3041,10 +3203,10 @@
         <v>0</v>
       </c>
       <c r="AX6" s="58" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G7" s="57"/>
       <c r="K7" s="2"/>
       <c r="Q7" s="47"/>
@@ -3065,12 +3227,12 @@
       <c r="AN7" s="58"/>
       <c r="AX7" s="58"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>500</v>
@@ -3122,22 +3284,22 @@
         <v>0.000104166666666667</v>
       </c>
       <c r="S8" s="61" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T8" s="61" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U8" s="61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="V8" s="58" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W8" s="58" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="X8" s="61" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y8" s="0" t="n">
         <v>0</v>
@@ -3146,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB8" s="0" t="n">
         <v>0</v>
@@ -3164,28 +3326,28 @@
         <v>0</v>
       </c>
       <c r="AG8" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH8" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI8" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ8" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK8" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL8" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM8" s="0" t="n">
         <v>0.35</v>
       </c>
       <c r="AN8" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO8" s="0" t="n">
         <v>0</v>
@@ -3221,12 +3383,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D9" s="56" t="n">
         <v>500</v>
@@ -3278,22 +3440,22 @@
         <v>0.000104166666666667</v>
       </c>
       <c r="S9" s="58" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U9" s="58" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="V9" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="W9" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="X9" s="58" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y9" s="56" t="n">
         <v>0</v>
@@ -3302,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB9" s="56" t="n">
         <v>0</v>
@@ -3320,28 +3482,28 @@
         <v>0</v>
       </c>
       <c r="AG9" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH9" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI9" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ9" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK9" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL9" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM9" s="56" t="n">
         <v>0.35</v>
       </c>
       <c r="AN9" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO9" s="56" t="n">
         <v>0</v>
@@ -3377,12 +3539,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D10" s="56" t="n">
         <v>500</v>
@@ -3434,22 +3596,22 @@
         <v>0.000104166666666667</v>
       </c>
       <c r="S10" s="58" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T10" s="61" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U10" s="61" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="V10" s="58" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W10" s="58" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="X10" s="58" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y10" s="56" t="n">
         <v>0</v>
@@ -3458,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB10" s="56" t="n">
         <v>0</v>
@@ -3476,28 +3638,28 @@
         <v>0</v>
       </c>
       <c r="AG10" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH10" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI10" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ10" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK10" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL10" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM10" s="56" t="n">
         <v>0.35</v>
       </c>
       <c r="AN10" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO10" s="56" t="n">
         <v>0</v>
@@ -3533,12 +3695,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D11" s="56" t="n">
         <v>500</v>
@@ -3590,22 +3752,22 @@
         <v>0.000104166666666667</v>
       </c>
       <c r="S11" s="58" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T11" s="61" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U11" s="61" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="V11" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="W11" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="X11" s="58" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y11" s="56" t="n">
         <v>0</v>
@@ -3614,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="AA11" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB11" s="56" t="n">
         <v>0</v>
@@ -3632,28 +3794,28 @@
         <v>0</v>
       </c>
       <c r="AG11" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH11" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI11" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ11" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK11" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL11" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM11" s="56" t="n">
         <v>0.35</v>
       </c>
       <c r="AN11" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO11" s="56" t="n">
         <v>0</v>
@@ -3689,12 +3851,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>5000</v>
@@ -3746,22 +3908,22 @@
         <v>1.04166666666667E-005</v>
       </c>
       <c r="S12" s="61" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U12" s="58" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="V12" s="58" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W12" s="58" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="X12" s="58" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y12" s="56" t="n">
         <v>0</v>
@@ -3770,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="AA12" s="58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB12" s="56" t="n">
         <v>0</v>
@@ -3788,28 +3950,28 @@
         <v>0</v>
       </c>
       <c r="AG12" s="58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH12" s="58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AI12" s="58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AJ12" s="58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AK12" s="58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL12" s="58" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM12" s="56" t="n">
         <v>0.35</v>
       </c>
       <c r="AN12" s="58" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AO12" s="56" t="n">
         <v>0</v>
@@ -3843,215 +4005,215 @@
         <v>1.04166666666667E-005</v>
       </c>
       <c r="AY12" s="61" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="46" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    </row>
+    <row r="31" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4066,21 +4228,22 @@
   </sheetPr>
   <dimension ref="A2:I21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.3019607843137"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.7372549019608"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.86224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86224489795918"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -4090,7 +4253,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="30" t="s">
         <v>69</v>
       </c>
@@ -4110,11 +4273,11 @@
         <v>74</v>
       </c>
       <c r="H3" s="66" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I3" s="67"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
@@ -4141,12 +4304,12 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>77</v>
@@ -4169,7 +4332,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="30" t="s">
         <v>82</v>
       </c>
@@ -4180,7 +4343,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
         <v>85</v>
       </c>
@@ -4200,10 +4363,10 @@
         <v>400</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
         <v>85</v>
       </c>
@@ -4218,10 +4381,10 @@
         <v>243</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
         <v>85</v>
       </c>
@@ -4241,10 +4404,10 @@
         <v>1.9</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="10">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
         <v>85</v>
       </c>
@@ -4253,15 +4416,15 @@
         <v>79</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>77</v>
@@ -4275,22 +4438,22 @@
         <v>876</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">0.26*365</f>
         <v>94.9</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="12">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>77</v>
@@ -4304,22 +4467,22 @@
         <v>0.019272</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H12" s="69" t="n">
         <f aca="false">365*5.3*10^{-4}</f>
         <v>0.19345</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>77</v>
@@ -4333,22 +4496,22 @@
         <v>4.38</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H13" s="56" t="n">
         <f aca="false">365*1*10^{-3}</f>
         <v>0.365</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>77</v>
@@ -4360,40 +4523,40 @@
         <v>10</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="17">
+    </row>
+    <row r="17" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.5</v>
@@ -4402,12 +4565,12 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.15" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0.5</v>
@@ -4416,15 +4579,15 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>